<commit_message>
add res boundary attack for SEED 314
</commit_message>
<xml_diff>
--- a/results/SEED_314/result.xlsx
+++ b/results/SEED_314/result.xlsx
@@ -800,124 +800,124 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4.296640396118164</v>
+        <v>4.296642780303955</v>
       </c>
       <c r="D4" t="n">
-        <v>3.290961503982544</v>
+        <v>3.290960550308228</v>
       </c>
       <c r="E4" t="n">
-        <v>4.276159503243186</v>
+        <v>4.276161670684814</v>
       </c>
       <c r="F4" t="n">
-        <v>4.522096937352961</v>
+        <v>4.522098627957431</v>
       </c>
       <c r="G4" t="n">
-        <v>5.037280689586293</v>
+        <v>5.037282250144265</v>
       </c>
       <c r="H4" t="n">
-        <v>5.799449877305464</v>
+        <v>5.799450614235618</v>
       </c>
       <c r="I4" t="n">
-        <v>6.740188295190984</v>
+        <v>6.740188446911898</v>
       </c>
       <c r="J4" t="n">
-        <v>9.555506988005204</v>
+        <v>9.555506446144797</v>
       </c>
       <c r="K4" t="n">
-        <v>12.58743765137412</v>
+        <v>12.58743736960671</v>
       </c>
       <c r="L4" t="n">
-        <v>24.25457672639327</v>
+        <v>24.25457631457936</v>
       </c>
       <c r="M4" t="n">
-        <v>4.30734092539007</v>
+        <v>4.307341879064387</v>
       </c>
       <c r="N4" t="n">
-        <v>4.319083430550315</v>
+        <v>4.319085684689608</v>
       </c>
       <c r="O4" t="n">
-        <v>4.331646269018</v>
+        <v>4.331647656180642</v>
       </c>
       <c r="P4" t="n">
-        <v>4.349610025232488</v>
+        <v>4.349611629139293</v>
       </c>
       <c r="Q4" t="n">
-        <v>4.371556108648127</v>
+        <v>4.371558319438588</v>
       </c>
       <c r="R4" t="n">
-        <v>4.447163061662153</v>
+        <v>4.447165229103782</v>
       </c>
       <c r="S4" t="n">
-        <v>4.575747836719859</v>
+        <v>4.575749614021995</v>
       </c>
       <c r="T4" t="n">
-        <v>5.592092730782249</v>
+        <v>5.592094031247226</v>
       </c>
       <c r="U4" t="n">
-        <v>4.30734092539007</v>
+        <v>4.307341879064387</v>
       </c>
       <c r="V4" t="n">
-        <v>4.319752086292613</v>
+        <v>4.319753256711093</v>
       </c>
       <c r="W4" t="n">
-        <v>4.332756996154785</v>
+        <v>4.332758903503418</v>
       </c>
       <c r="X4" t="n">
-        <v>4.35109940442172</v>
+        <v>4.351101355119185</v>
       </c>
       <c r="Y4" t="n">
-        <v>4.373739979483864</v>
+        <v>4.373741279948842</v>
       </c>
       <c r="Z4" t="n">
-        <v>4.430071874098345</v>
+        <v>4.43007382479581</v>
       </c>
       <c r="AA4" t="n">
-        <v>4.583161093971946</v>
+        <v>4.583163781599565</v>
       </c>
       <c r="AB4" t="n">
-        <v>5.983649470589378</v>
+        <v>5.983651768077504</v>
       </c>
       <c r="AC4" t="n">
-        <v>5.36815357208252</v>
+        <v>5.368155956268311</v>
       </c>
       <c r="AD4" t="n">
-        <v>6.663228988647461</v>
+        <v>6.663232326507568</v>
       </c>
       <c r="AE4" t="n">
-        <v>8.028472900390625</v>
+        <v>8.028476715087891</v>
       </c>
       <c r="AF4" t="n">
-        <v>9.414920806884766</v>
+        <v>9.414924621582031</v>
       </c>
       <c r="AG4" t="n">
-        <v>10.81547451019287</v>
+        <v>10.8154764175415</v>
       </c>
       <c r="AH4" t="n">
-        <v>14.32437705993652</v>
+        <v>14.32437992095947</v>
       </c>
       <c r="AI4" t="n">
-        <v>17.83636665344238</v>
+        <v>17.83637046813965</v>
       </c>
       <c r="AJ4" t="n">
-        <v>31.85391235351562</v>
+        <v>31.85391426086426</v>
       </c>
       <c r="AK4" t="n">
-        <v>5.693411827087402</v>
+        <v>5.693414211273193</v>
       </c>
       <c r="AL4" t="n">
-        <v>7.092088222503662</v>
+        <v>7.092090129852295</v>
       </c>
       <c r="AM4" t="n">
-        <v>8.492356300354004</v>
+        <v>8.492359161376953</v>
       </c>
       <c r="AN4" t="n">
-        <v>9.894145965576172</v>
+        <v>9.894147872924805</v>
       </c>
       <c r="AO4" t="n">
-        <v>11.29704761505127</v>
+        <v>11.2970495223999</v>
       </c>
       <c r="AP4" t="n">
-        <v>14.80758666992188</v>
+        <v>14.80758762359619</v>
       </c>
       <c r="AQ4" t="n">
         <v>18.31450653076172</v>
@@ -934,130 +934,130 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5.432599194003322</v>
+        <v>5.432601125015577</v>
       </c>
       <c r="D5" t="n">
-        <v>4.361214635852676</v>
+        <v>4.361213761165698</v>
       </c>
       <c r="E5" t="n">
-        <v>5.466387330672015</v>
+        <v>5.466389803429237</v>
       </c>
       <c r="F5" t="n">
-        <v>5.81262829572588</v>
+        <v>5.812629886611811</v>
       </c>
       <c r="G5" t="n">
-        <v>6.418926052930994</v>
+        <v>6.418928135836604</v>
       </c>
       <c r="H5" t="n">
-        <v>7.220209614045022</v>
+        <v>7.220210843008489</v>
       </c>
       <c r="I5" t="n">
-        <v>8.158476304342873</v>
+        <v>8.158476964662221</v>
       </c>
       <c r="J5" t="n">
-        <v>10.84780548847591</v>
+        <v>10.84780572993084</v>
       </c>
       <c r="K5" t="n">
-        <v>13.77515879826594</v>
+        <v>13.77515935274668</v>
       </c>
       <c r="L5" t="n">
-        <v>25.6819950746461</v>
+        <v>25.68199516791736</v>
       </c>
       <c r="M5" t="n">
-        <v>5.443312690815651</v>
+        <v>5.443314182129007</v>
       </c>
       <c r="N5" t="n">
-        <v>5.45637114512457</v>
+        <v>5.456373847261611</v>
       </c>
       <c r="O5" t="n">
-        <v>5.471534939608696</v>
+        <v>5.471536540425452</v>
       </c>
       <c r="P5" t="n">
-        <v>5.491460493286504</v>
+        <v>5.491462029365739</v>
       </c>
       <c r="Q5" t="n">
-        <v>5.518205219910642</v>
+        <v>5.518206845360411</v>
       </c>
       <c r="R5" t="n">
-        <v>5.61036852857029</v>
+        <v>5.610370521486991</v>
       </c>
       <c r="S5" t="n">
-        <v>5.7856315463905</v>
+        <v>5.785633268519052</v>
       </c>
       <c r="T5" t="n">
-        <v>7.281358493850537</v>
+        <v>7.281359917844471</v>
       </c>
       <c r="U5" t="n">
-        <v>5.443312690815651</v>
+        <v>5.443314182129007</v>
       </c>
       <c r="V5" t="n">
-        <v>5.45642273944329</v>
+        <v>5.456424165127976</v>
       </c>
       <c r="W5" t="n">
-        <v>5.471408551961235</v>
+        <v>5.471410536907904</v>
       </c>
       <c r="X5" t="n">
-        <v>5.491118482676341</v>
+        <v>5.491120457618108</v>
       </c>
       <c r="Y5" t="n">
-        <v>5.51775026093616</v>
+        <v>5.517751860554689</v>
       </c>
       <c r="Z5" t="n">
-        <v>5.586149879004428</v>
+        <v>5.586151868065143</v>
       </c>
       <c r="AA5" t="n">
-        <v>5.792074078316268</v>
+        <v>5.79207649009311</v>
       </c>
       <c r="AB5" t="n">
-        <v>7.708551129915423</v>
+        <v>7.70855319693605</v>
       </c>
       <c r="AC5" t="n">
-        <v>6.475898662638995</v>
+        <v>6.475901018881284</v>
       </c>
       <c r="AD5" t="n">
-        <v>7.633653826697253</v>
+        <v>7.633656825022776</v>
       </c>
       <c r="AE5" t="n">
-        <v>8.86264381453417</v>
+        <v>8.862646827503761</v>
       </c>
       <c r="AF5" t="n">
-        <v>10.13791614435629</v>
+        <v>10.13791953087766</v>
       </c>
       <c r="AG5" t="n">
-        <v>11.44473121390772</v>
+        <v>11.44473321379581</v>
       </c>
       <c r="AH5" t="n">
-        <v>14.79537553450507</v>
+        <v>14.79537862846928</v>
       </c>
       <c r="AI5" t="n">
-        <v>18.20959598635643</v>
+        <v>18.20959850021583</v>
       </c>
       <c r="AJ5" t="n">
-        <v>32.05993380324966</v>
+        <v>32.05993761081539</v>
       </c>
       <c r="AK5" t="n">
-        <v>6.58099983804955</v>
+        <v>6.581002446488194</v>
       </c>
       <c r="AL5" t="n">
-        <v>7.814252244903069</v>
+        <v>7.81425395350404</v>
       </c>
       <c r="AM5" t="n">
-        <v>9.098701937810965</v>
+        <v>9.098704872611636</v>
       </c>
       <c r="AN5" t="n">
-        <v>10.41594915334828</v>
+        <v>10.41595098452894</v>
       </c>
       <c r="AO5" t="n">
-        <v>11.75528549464227</v>
+        <v>11.75528679267865</v>
       </c>
       <c r="AP5" t="n">
-        <v>15.16115114858996</v>
+        <v>15.16115366468977</v>
       </c>
       <c r="AQ5" t="n">
-        <v>18.60708473391041</v>
+        <v>18.60708637401563</v>
       </c>
       <c r="AR5" t="n">
-        <v>32.41387890855455</v>
+        <v>32.41388079154901</v>
       </c>
     </row>
     <row r="6">
@@ -1074,67 +1074,67 @@
         <v>0.9996763467788696</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9996130466461182</v>
+        <v>0.9996131658554077</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9995262026786804</v>
+        <v>0.9995262622833252</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9993757605552673</v>
+        <v>0.9993756413459778</v>
       </c>
       <c r="H6" t="n">
         <v>0.9991620779037476</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9988858103752136</v>
+        <v>0.9988858699798584</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9979274868965149</v>
+        <v>0.9979276061058044</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9965997934341431</v>
+        <v>0.9966000318527222</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9880918264389038</v>
+        <v>0.9880918860435486</v>
       </c>
       <c r="M6" t="n">
-        <v>0.9996358752250671</v>
+        <v>0.9996361136436462</v>
       </c>
       <c r="N6" t="n">
-        <v>0.9996355175971985</v>
+        <v>0.999635636806488</v>
       </c>
       <c r="O6" t="n">
-        <v>0.9996349811553955</v>
+        <v>0.9996350407600403</v>
       </c>
       <c r="P6" t="n">
-        <v>0.9996337294578552</v>
+        <v>0.9996338486671448</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.9996317028999329</v>
+        <v>0.999631941318512</v>
       </c>
       <c r="R6" t="n">
-        <v>0.9996233582496643</v>
+        <v>0.9996234774589539</v>
       </c>
       <c r="S6" t="n">
-        <v>0.9996038675308228</v>
+        <v>0.9996037483215332</v>
       </c>
       <c r="T6" t="n">
         <v>0.9994052648544312</v>
       </c>
       <c r="U6" t="n">
-        <v>0.9996358752250671</v>
+        <v>0.9996361136436462</v>
       </c>
       <c r="V6" t="n">
-        <v>0.9996353983879089</v>
+        <v>0.9996355175971985</v>
       </c>
       <c r="W6" t="n">
-        <v>0.9996346235275269</v>
+        <v>0.999634861946106</v>
       </c>
       <c r="X6" t="n">
-        <v>0.9996334314346313</v>
+        <v>0.9996335506439209</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.9996311068534851</v>
+        <v>0.9996312856674194</v>
       </c>
       <c r="Z6" t="n">
         <v>0.9996243715286255</v>
@@ -1143,55 +1143,55 @@
         <v>0.9996022582054138</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.9994092583656311</v>
+        <v>0.9994093775749207</v>
       </c>
       <c r="AC6" t="n">
         <v>0.9995546936988831</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.999445378780365</v>
+        <v>0.9994454979896545</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.99930739402771</v>
+        <v>0.9993075728416443</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.9991394281387329</v>
+        <v>0.9991394877433777</v>
       </c>
       <c r="AG6" t="n">
         <v>0.9989404082298279</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.9982986450195312</v>
+        <v>0.9982985854148865</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.9974371790885925</v>
+        <v>0.9974369406700134</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.9914015531539917</v>
+        <v>0.9914016127586365</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.9994690418243408</v>
+        <v>0.9994689226150513</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.9992448091506958</v>
+        <v>0.9992449283599854</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.9989621639251709</v>
+        <v>0.9989624619483948</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.9986199140548706</v>
+        <v>0.9986200332641602</v>
       </c>
       <c r="AO6" t="n">
         <v>0.9982166886329651</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.9969327449798584</v>
+        <v>0.9969328641891479</v>
       </c>
       <c r="AQ6" t="n">
         <v>0.9952425956726074</v>
       </c>
       <c r="AR6" t="n">
-        <v>0.9842365384101868</v>
+        <v>0.9842366576194763</v>
       </c>
     </row>
     <row r="7">
@@ -1206,127 +1206,127 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3.978105783462524</v>
+        <v>3.978102207183838</v>
       </c>
       <c r="D7" t="n">
-        <v>2.80927586555481</v>
+        <v>2.809282541275024</v>
       </c>
       <c r="E7" t="n">
-        <v>3.633406855843284</v>
+        <v>3.633402781053023</v>
       </c>
       <c r="F7" t="n">
-        <v>3.36254375631159</v>
+        <v>3.362540808590976</v>
       </c>
       <c r="G7" t="n">
-        <v>3.16169565374201</v>
+        <v>3.161691752347079</v>
       </c>
       <c r="H7" t="n">
-        <v>3.08661582253196</v>
+        <v>3.086614608764648</v>
       </c>
       <c r="I7" t="n">
-        <v>3.151815501126376</v>
+        <v>3.151814937591553</v>
       </c>
       <c r="J7" t="n">
-        <v>3.794893611561168</v>
+        <v>3.794894868677313</v>
       </c>
       <c r="K7" t="n">
-        <v>4.966498353264549</v>
+        <v>4.966500629078258</v>
       </c>
       <c r="L7" t="n">
-        <v>9.846793933348222</v>
+        <v>9.846794908696955</v>
       </c>
       <c r="M7" t="n">
-        <v>3.896388140591708</v>
+        <v>3.896383588964289</v>
       </c>
       <c r="N7" t="n">
-        <v>3.827009851282293</v>
+        <v>3.827005689794367</v>
       </c>
       <c r="O7" t="n">
-        <v>3.769885149869052</v>
+        <v>3.769881595264782</v>
       </c>
       <c r="P7" t="n">
-        <v>3.723149299621582</v>
+        <v>3.723146308552135</v>
       </c>
       <c r="Q7" t="n">
-        <v>3.6947565945712</v>
+        <v>3.694752303036776</v>
       </c>
       <c r="R7" t="n">
-        <v>3.693013364618475</v>
+        <v>3.693010460246693</v>
       </c>
       <c r="S7" t="n">
-        <v>3.805766690861095</v>
+        <v>3.805764219977639</v>
       </c>
       <c r="T7" t="n">
-        <v>5.439262801950628</v>
+        <v>5.439261133020574</v>
       </c>
       <c r="U7" t="n">
-        <v>3.633406855843284</v>
+        <v>3.633402781053023</v>
       </c>
       <c r="V7" t="n">
-        <v>3.360595486380837</v>
+        <v>3.360592538660223</v>
       </c>
       <c r="W7" t="n">
-        <v>3.155259652571245</v>
+        <v>3.155258438803933</v>
       </c>
       <c r="X7" t="n">
-        <v>3.076050281524658</v>
+        <v>3.076048330827193</v>
       </c>
       <c r="Y7" t="n">
-        <v>3.138622544028542</v>
+        <v>3.138620593331077</v>
       </c>
       <c r="Z7" t="n">
-        <v>3.599713628942316</v>
+        <v>3.599714149128307</v>
       </c>
       <c r="AA7" t="n">
-        <v>4.998368003151634</v>
+        <v>4.99836930361661</v>
       </c>
       <c r="AB7" t="n">
-        <v>10.00202475894581</v>
+        <v>10.00202614610845</v>
       </c>
       <c r="AC7" t="n">
-        <v>5.348810195922852</v>
+        <v>5.348807811737061</v>
       </c>
       <c r="AD7" t="n">
-        <v>6.756837368011475</v>
+        <v>6.756833076477051</v>
       </c>
       <c r="AE7" t="n">
-        <v>8.167000770568848</v>
+        <v>8.166996002197266</v>
       </c>
       <c r="AF7" t="n">
-        <v>9.579092979431152</v>
+        <v>9.579090118408203</v>
       </c>
       <c r="AG7" t="n">
-        <v>10.99174880981445</v>
+        <v>10.9917459487915</v>
       </c>
       <c r="AH7" t="n">
-        <v>14.52614116668701</v>
+        <v>14.52613925933838</v>
       </c>
       <c r="AI7" t="n">
         <v>18.05896186828613</v>
       </c>
       <c r="AJ7" t="n">
-        <v>32.15625</v>
+        <v>32.15625381469727</v>
       </c>
       <c r="AK7" t="n">
-        <v>5.599724292755127</v>
+        <v>5.599720478057861</v>
       </c>
       <c r="AL7" t="n">
-        <v>7.224311351776123</v>
+        <v>7.224307060241699</v>
       </c>
       <c r="AM7" t="n">
-        <v>8.851334571838379</v>
+        <v>8.851329803466797</v>
       </c>
       <c r="AN7" t="n">
-        <v>10.48008155822754</v>
+        <v>10.48007774353027</v>
       </c>
       <c r="AO7" t="n">
-        <v>12.1090784072876</v>
+        <v>12.10907363891602</v>
       </c>
       <c r="AP7" t="n">
-        <v>16.18157196044922</v>
+        <v>16.18157005310059</v>
       </c>
       <c r="AQ7" t="n">
-        <v>20.24405670166016</v>
+        <v>20.24405479431152</v>
       </c>
       <c r="AR7" t="n">
         <v>36.36486434936523</v>
@@ -1340,127 +1340,127 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.99584731268922</v>
+        <v>4.99584406750024</v>
       </c>
       <c r="D8" t="n">
-        <v>3.831831402870488</v>
+        <v>3.831838122681789</v>
       </c>
       <c r="E8" t="n">
-        <v>4.628058018035543</v>
+        <v>4.628053616403399</v>
       </c>
       <c r="F8" t="n">
-        <v>4.360469793936431</v>
+        <v>4.360466655702962</v>
       </c>
       <c r="G8" t="n">
-        <v>4.21215569434119</v>
+        <v>4.212151445483689</v>
       </c>
       <c r="H8" t="n">
-        <v>4.196324775282037</v>
+        <v>4.196323471316014</v>
       </c>
       <c r="I8" t="n">
-        <v>4.314480724027921</v>
+        <v>4.314479509951848</v>
       </c>
       <c r="J8" t="n">
-        <v>5.087424833990542</v>
+        <v>5.087425261657057</v>
       </c>
       <c r="K8" t="n">
-        <v>6.299937454743915</v>
+        <v>6.299938304073287</v>
       </c>
       <c r="L8" t="n">
-        <v>11.98425669165284</v>
+        <v>11.98425784880416</v>
       </c>
       <c r="M8" t="n">
-        <v>4.898767948102054</v>
+        <v>4.898762672857097</v>
       </c>
       <c r="N8" t="n">
-        <v>4.817498038488653</v>
+        <v>4.817494107998249</v>
       </c>
       <c r="O8" t="n">
-        <v>4.752784713182647</v>
+        <v>4.752780440694719</v>
       </c>
       <c r="P8" t="n">
-        <v>4.708365058400861</v>
+        <v>4.708361744611162</v>
       </c>
       <c r="Q8" t="n">
-        <v>4.684232391861924</v>
+        <v>4.684228115988055</v>
       </c>
       <c r="R8" t="n">
-        <v>4.721148607795148</v>
+        <v>4.721146224831054</v>
       </c>
       <c r="S8" t="n">
-        <v>4.932074497926421</v>
+        <v>4.93207274117709</v>
       </c>
       <c r="T8" t="n">
-        <v>7.00312392678391</v>
+        <v>7.003122129316608</v>
       </c>
       <c r="U8" t="n">
-        <v>4.628058018035543</v>
+        <v>4.628053616403399</v>
       </c>
       <c r="V8" t="n">
-        <v>4.358865084481086</v>
+        <v>4.358861592354431</v>
       </c>
       <c r="W8" t="n">
-        <v>4.208385707587022</v>
+        <v>4.208384048343535</v>
       </c>
       <c r="X8" t="n">
-        <v>4.198809106526398</v>
+        <v>4.198807135337124</v>
       </c>
       <c r="Y8" t="n">
-        <v>4.324428448817866</v>
+        <v>4.324426678518335</v>
       </c>
       <c r="Z8" t="n">
-        <v>4.916426805770438</v>
+        <v>4.916426623969624</v>
       </c>
       <c r="AA8" t="n">
-        <v>6.361060196008126</v>
+        <v>6.361061287312943</v>
       </c>
       <c r="AB8" t="n">
-        <v>12.10998147714421</v>
+        <v>12.10998277590184</v>
       </c>
       <c r="AC8" t="n">
-        <v>6.152557349962703</v>
+        <v>6.15255362985264</v>
       </c>
       <c r="AD8" t="n">
-        <v>7.399963286025241</v>
+        <v>7.399958646504094</v>
       </c>
       <c r="AE8" t="n">
-        <v>8.70007073384612</v>
+        <v>8.700065472235908</v>
       </c>
       <c r="AF8" t="n">
-        <v>10.03299648019384</v>
+        <v>10.03299343847218</v>
       </c>
       <c r="AG8" t="n">
-        <v>11.38689228534145</v>
+        <v>11.38688893526337</v>
       </c>
       <c r="AH8" t="n">
-        <v>14.82736400263383</v>
+        <v>14.82736297353725</v>
       </c>
       <c r="AI8" t="n">
-        <v>18.30808077142995</v>
+        <v>18.30807827109303</v>
       </c>
       <c r="AJ8" t="n">
-        <v>32.35111631091731</v>
+        <v>32.35111819756487</v>
       </c>
       <c r="AK8" t="n">
-        <v>6.348050468527843</v>
+        <v>6.348046562519222</v>
       </c>
       <c r="AL8" t="n">
-        <v>7.807878515893117</v>
+        <v>7.807874363044771</v>
       </c>
       <c r="AM8" t="n">
-        <v>9.326101725848742</v>
+        <v>9.326097226468265</v>
       </c>
       <c r="AN8" t="n">
-        <v>10.87844127709207</v>
+        <v>10.87843741976764</v>
       </c>
       <c r="AO8" t="n">
-        <v>12.45173237096292</v>
+        <v>12.45172685650406</v>
       </c>
       <c r="AP8" t="n">
-        <v>16.43666358821368</v>
+        <v>16.43665987485891</v>
       </c>
       <c r="AQ8" t="n">
-        <v>20.45129190482039</v>
+        <v>20.4512896665085</v>
       </c>
       <c r="AR8" t="n">
         <v>36.52752400266989</v>
@@ -1480,91 +1480,91 @@
         <v>0.9998423457145691</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9997787475585938</v>
+        <v>0.9997788667678833</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9997707605361938</v>
+        <v>0.9997708201408386</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9997519254684448</v>
+        <v>0.9997519850730896</v>
       </c>
       <c r="H9" t="n">
-        <v>0.999722421169281</v>
+        <v>0.9997225403785706</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9996819496154785</v>
+        <v>0.9996820688247681</v>
       </c>
       <c r="J9" t="n">
-        <v>0.9995357394218445</v>
+        <v>0.999535858631134</v>
       </c>
       <c r="K9" t="n">
-        <v>0.9993228912353516</v>
+        <v>0.9993230700492859</v>
       </c>
       <c r="L9" t="n">
-        <v>0.9978935122489929</v>
+        <v>0.9978935718536377</v>
       </c>
       <c r="M9" t="n">
         <v>0.9997784495353699</v>
       </c>
       <c r="N9" t="n">
-        <v>0.9997782707214355</v>
+        <v>0.9997783899307251</v>
       </c>
       <c r="O9" t="n">
-        <v>0.9997758269309998</v>
+        <v>0.9997759461402893</v>
       </c>
       <c r="P9" t="n">
-        <v>0.9997705817222595</v>
+        <v>0.9997707009315491</v>
       </c>
       <c r="Q9" t="n">
         <v>0.9997627139091492</v>
       </c>
       <c r="R9" t="n">
-        <v>0.9997304677963257</v>
+        <v>0.99973064661026</v>
       </c>
       <c r="S9" t="n">
-        <v>0.9996760487556458</v>
+        <v>0.9996761679649353</v>
       </c>
       <c r="T9" t="n">
-        <v>0.9992221593856812</v>
+        <v>0.9992222785949707</v>
       </c>
       <c r="U9" t="n">
-        <v>0.9997787475585938</v>
+        <v>0.9997788667678833</v>
       </c>
       <c r="V9" t="n">
-        <v>0.9997711777687073</v>
+        <v>0.9997713565826416</v>
       </c>
       <c r="W9" t="n">
-        <v>0.999752938747406</v>
+        <v>0.9997530579566956</v>
       </c>
       <c r="X9" t="n">
-        <v>0.9997228384017944</v>
+        <v>0.999722957611084</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.999681293964386</v>
+        <v>0.9996813535690308</v>
       </c>
       <c r="Z9" t="n">
         <v>0.9995651841163635</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.999302864074707</v>
+        <v>0.9993029832839966</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.997722327709198</v>
+        <v>0.9977225065231323</v>
       </c>
       <c r="AC9" t="n">
         <v>0.9996587634086609</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.9994903802871704</v>
+        <v>0.99949049949646</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.9992696642875671</v>
+        <v>0.9992697834968567</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.9989950656890869</v>
+        <v>0.9989951848983765</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.9986658692359924</v>
+        <v>0.9986661076545715</v>
       </c>
       <c r="AH9" t="n">
         <v>0.9975932240486145</v>
@@ -1579,7 +1579,7 @@
         <v>0.9996665716171265</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.9995042681694031</v>
+        <v>0.999504566192627</v>
       </c>
       <c r="AM9" t="n">
         <v>0.9992876648902893</v>
@@ -1588,16 +1588,16 @@
         <v>0.9990139007568359</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.9986819624900818</v>
+        <v>0.9986820816993713</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.997581958770752</v>
+        <v>0.9975820779800415</v>
       </c>
       <c r="AQ9" t="n">
-        <v>0.9960711002349854</v>
+        <v>0.9960712194442749</v>
       </c>
       <c r="AR9" t="n">
-        <v>0.9851985573768616</v>
+        <v>0.9851986169815063</v>
       </c>
     </row>
     <row r="10">
@@ -1612,85 +1612,85 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3.359910488128662</v>
+        <v>3.359910011291504</v>
       </c>
       <c r="D10" t="n">
-        <v>2.01140570640564</v>
+        <v>2.011407375335693</v>
       </c>
       <c r="E10" t="n">
-        <v>3.329338203776966</v>
+        <v>3.329338550567627</v>
       </c>
       <c r="F10" t="n">
-        <v>3.314596869728782</v>
+        <v>3.314596349542791</v>
       </c>
       <c r="G10" t="n">
         <v>3.31283036145297</v>
       </c>
       <c r="H10" t="n">
-        <v>3.320879546078769</v>
+        <v>3.320878939195113</v>
       </c>
       <c r="I10" t="n">
-        <v>3.343091531233354</v>
+        <v>3.343091878024015</v>
       </c>
       <c r="J10" t="n">
-        <v>3.455863432450728</v>
+        <v>3.455863519148393</v>
       </c>
       <c r="K10" t="n">
-        <v>3.634256319566207</v>
+        <v>3.634255474263972</v>
       </c>
       <c r="L10" t="n">
-        <v>4.987139355052602</v>
+        <v>4.98713900826194</v>
       </c>
       <c r="M10" t="n">
-        <v>3.085448438471014</v>
+        <v>3.085448395122181</v>
       </c>
       <c r="N10" t="n">
-        <v>2.873865951191295</v>
+        <v>2.87386603788896</v>
       </c>
       <c r="O10" t="n">
-        <v>2.761151660572399</v>
+        <v>2.761152267456055</v>
       </c>
       <c r="P10" t="n">
-        <v>2.777359745719216</v>
+        <v>2.777360049161044</v>
       </c>
       <c r="Q10" t="n">
-        <v>2.928339177911932</v>
+        <v>2.928339047865434</v>
       </c>
       <c r="R10" t="n">
-        <v>3.767810041254217</v>
+        <v>3.767809369347312</v>
       </c>
       <c r="S10" t="n">
-        <v>4.950884819030762</v>
+        <v>4.950884667309848</v>
       </c>
       <c r="T10" t="n">
-        <v>9.407238266684793</v>
+        <v>9.407238223335959</v>
       </c>
       <c r="U10" t="n">
-        <v>3.329338203776966</v>
+        <v>3.329338550567627</v>
       </c>
       <c r="V10" t="n">
-        <v>3.314182714982466</v>
+        <v>3.314182411540638</v>
       </c>
       <c r="W10" t="n">
-        <v>3.314846168864857</v>
+        <v>3.314846775748513</v>
       </c>
       <c r="X10" t="n">
-        <v>3.325186035849832</v>
+        <v>3.325186165896329</v>
       </c>
       <c r="Y10" t="n">
-        <v>3.347530928525058</v>
+        <v>3.347531535408713</v>
       </c>
       <c r="Z10" t="n">
-        <v>3.416182366284457</v>
+        <v>3.41618292981928</v>
       </c>
       <c r="AA10" t="n">
-        <v>3.590754357251254</v>
+        <v>3.590754682367498</v>
       </c>
       <c r="AB10" t="n">
-        <v>5.164258653467352</v>
+        <v>5.164258328351107</v>
       </c>
       <c r="AC10" t="n">
-        <v>4.694666862487793</v>
+        <v>4.694665431976318</v>
       </c>
       <c r="AD10" t="n">
         <v>6.048988819122314</v>
@@ -1699,16 +1699,16 @@
         <v>7.410304069519043</v>
       </c>
       <c r="AF10" t="n">
-        <v>8.771474838256836</v>
+        <v>8.771475791931152</v>
       </c>
       <c r="AG10" t="n">
         <v>10.13043689727783</v>
       </c>
       <c r="AH10" t="n">
-        <v>13.5243558883667</v>
+        <v>13.52435398101807</v>
       </c>
       <c r="AI10" t="n">
-        <v>16.9118824005127</v>
+        <v>16.91188049316406</v>
       </c>
       <c r="AJ10" t="n">
         <v>30.2991771697998</v>
@@ -1717,13 +1717,13 @@
         <v>4.860269069671631</v>
       </c>
       <c r="AL10" t="n">
-        <v>6.361564159393311</v>
+        <v>6.361562728881836</v>
       </c>
       <c r="AM10" t="n">
-        <v>7.863556385040283</v>
+        <v>7.8635573387146</v>
       </c>
       <c r="AN10" t="n">
-        <v>9.364760398864746</v>
+        <v>9.364761352539062</v>
       </c>
       <c r="AO10" t="n">
         <v>10.86281681060791</v>
@@ -1746,100 +1746,100 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4.251468180458737</v>
+        <v>4.251467956142266</v>
       </c>
       <c r="D11" t="n">
-        <v>2.959708167458988</v>
+        <v>2.959709778553735</v>
       </c>
       <c r="E11" t="n">
-        <v>4.217885946850734</v>
+        <v>4.217885998075343</v>
       </c>
       <c r="F11" t="n">
-        <v>4.195777412024704</v>
+        <v>4.195776718357958</v>
       </c>
       <c r="G11" t="n">
-        <v>4.186025051182668</v>
+        <v>4.186024798034071</v>
       </c>
       <c r="H11" t="n">
-        <v>4.191362812486752</v>
+        <v>4.19136209514341</v>
       </c>
       <c r="I11" t="n">
-        <v>4.211358444382471</v>
+        <v>4.211358818812883</v>
       </c>
       <c r="J11" t="n">
-        <v>4.331165857349924</v>
+        <v>4.331166555187986</v>
       </c>
       <c r="K11" t="n">
-        <v>4.582668565179659</v>
+        <v>4.582667497662736</v>
       </c>
       <c r="L11" t="n">
-        <v>6.659679276595662</v>
+        <v>6.659678812896951</v>
       </c>
       <c r="M11" t="n">
-        <v>3.966130409061309</v>
+        <v>3.966130539208959</v>
       </c>
       <c r="N11" t="n">
-        <v>3.789747237409151</v>
+        <v>3.78974719773709</v>
       </c>
       <c r="O11" t="n">
-        <v>3.738800722176121</v>
+        <v>3.738801447329711</v>
       </c>
       <c r="P11" t="n">
-        <v>3.818171459516012</v>
+        <v>3.818171822482197</v>
       </c>
       <c r="Q11" t="n">
-        <v>4.018618721093405</v>
+        <v>4.018619250876186</v>
       </c>
       <c r="R11" t="n">
-        <v>4.913201727966109</v>
+        <v>4.913200742670999</v>
       </c>
       <c r="S11" t="n">
-        <v>6.13521825157022</v>
+        <v>6.135218105122711</v>
       </c>
       <c r="T11" t="n">
-        <v>11.48854566740785</v>
+        <v>11.48854509713922</v>
       </c>
       <c r="U11" t="n">
-        <v>4.217885946850734</v>
+        <v>4.217885998075343</v>
       </c>
       <c r="V11" t="n">
-        <v>4.195607743269511</v>
+        <v>4.195607008208654</v>
       </c>
       <c r="W11" t="n">
-        <v>4.186023926767787</v>
+        <v>4.186024363539522</v>
       </c>
       <c r="X11" t="n">
-        <v>4.192051653592366</v>
+        <v>4.192051977819512</v>
       </c>
       <c r="Y11" t="n">
-        <v>4.211285916886825</v>
+        <v>4.211286013960021</v>
       </c>
       <c r="Z11" t="n">
-        <v>4.278870134503698</v>
+        <v>4.278870875642674</v>
       </c>
       <c r="AA11" t="n">
-        <v>4.523556816679068</v>
+        <v>4.523556803286723</v>
       </c>
       <c r="AB11" t="n">
-        <v>6.765895474009073</v>
+        <v>6.765895422002088</v>
       </c>
       <c r="AC11" t="n">
-        <v>5.376969797127258</v>
+        <v>5.376969087676088</v>
       </c>
       <c r="AD11" t="n">
-        <v>6.593360925558204</v>
+        <v>6.593360346991752</v>
       </c>
       <c r="AE11" t="n">
-        <v>7.859019216443843</v>
+        <v>7.859019459139343</v>
       </c>
       <c r="AF11" t="n">
-        <v>9.153033944846255</v>
+        <v>9.153035195152011</v>
       </c>
       <c r="AG11" t="n">
         <v>10.46334544495166</v>
       </c>
       <c r="AH11" t="n">
-        <v>13.78171114679846</v>
+        <v>13.78171003962175</v>
       </c>
       <c r="AI11" t="n">
         <v>17.12962468205439</v>
@@ -1851,22 +1851,22 @@
         <v>5.509160822331165</v>
       </c>
       <c r="AL11" t="n">
-        <v>6.866918912285217</v>
+        <v>6.866918079008122</v>
       </c>
       <c r="AM11" t="n">
-        <v>8.275924179238704</v>
+        <v>8.275925101116906</v>
       </c>
       <c r="AN11" t="n">
-        <v>9.712937558012991</v>
+        <v>9.712937950756913</v>
       </c>
       <c r="AO11" t="n">
-        <v>11.16495189500927</v>
+        <v>11.16495121167496</v>
       </c>
       <c r="AP11" t="n">
-        <v>14.83156366543052</v>
+        <v>14.83156263662533</v>
       </c>
       <c r="AQ11" t="n">
-        <v>18.51499125365839</v>
+        <v>18.51499290192149</v>
       </c>
       <c r="AR11" t="n">
         <v>33.11585405872937</v>
@@ -1880,25 +1880,25 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.9998025298118591</v>
+        <v>0.9998026490211487</v>
       </c>
       <c r="D12" t="n">
         <v>0.9998846650123596</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9998038411140442</v>
+        <v>0.999803900718689</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9998035430908203</v>
+        <v>0.9998037815093994</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9998016357421875</v>
+        <v>0.9998017549514771</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9997976422309875</v>
+        <v>0.9997977018356323</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9997919201850891</v>
+        <v>0.9997920393943787</v>
       </c>
       <c r="J12" t="n">
         <v>0.9997687935829163</v>
@@ -1907,70 +1907,70 @@
         <v>0.9997292160987854</v>
       </c>
       <c r="L12" t="n">
-        <v>0.9993777871131897</v>
+        <v>0.9993779063224792</v>
       </c>
       <c r="M12" t="n">
-        <v>0.9998025894165039</v>
+        <v>0.9998027086257935</v>
       </c>
       <c r="N12" t="n">
-        <v>0.9997932314872742</v>
+        <v>0.9997934699058533</v>
       </c>
       <c r="O12" t="n">
-        <v>0.9997749924659729</v>
+        <v>0.9997751116752625</v>
       </c>
       <c r="P12" t="n">
-        <v>0.9997473955154419</v>
+        <v>0.9997475147247314</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.9997106194496155</v>
+        <v>0.999710738658905</v>
       </c>
       <c r="R12" t="n">
-        <v>0.9995803236961365</v>
+        <v>0.999580442905426</v>
       </c>
       <c r="S12" t="n">
-        <v>0.9993936419487</v>
+        <v>0.9993937611579895</v>
       </c>
       <c r="T12" t="n">
-        <v>0.9981426596641541</v>
+        <v>0.9981425404548645</v>
       </c>
       <c r="U12" t="n">
-        <v>0.9998038411140442</v>
+        <v>0.999803900718689</v>
       </c>
       <c r="V12" t="n">
         <v>0.9998032450675964</v>
       </c>
       <c r="W12" t="n">
-        <v>0.9998008012771606</v>
+        <v>0.999800980091095</v>
       </c>
       <c r="X12" t="n">
-        <v>0.9997965097427368</v>
+        <v>0.9997968077659607</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.9997904896736145</v>
+        <v>0.9997906088829041</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.9997740983963013</v>
+        <v>0.9997743368148804</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.9997351765632629</v>
+        <v>0.9997352957725525</v>
       </c>
       <c r="AB12" t="n">
         <v>0.9994234442710876</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.9996980428695679</v>
+        <v>0.9996981620788574</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.9995487332344055</v>
+        <v>0.9995488524436951</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.9993531703948975</v>
+        <v>0.999353289604187</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.9991107583045959</v>
+        <v>0.9991108775138855</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.998821496963501</v>
+        <v>0.9988216757774353</v>
       </c>
       <c r="AH12" t="n">
         <v>0.9978824257850647</v>
@@ -1979,13 +1979,13 @@
         <v>0.9966186285018921</v>
       </c>
       <c r="AJ12" t="n">
-        <v>0.988116443157196</v>
+        <v>0.9881165623664856</v>
       </c>
       <c r="AK12" t="n">
-        <v>0.9996857047080994</v>
+        <v>0.9996858239173889</v>
       </c>
       <c r="AL12" t="n">
-        <v>0.9995155334472656</v>
+        <v>0.9995156526565552</v>
       </c>
       <c r="AM12" t="n">
         <v>0.9992904663085938</v>
@@ -1997,7 +1997,7 @@
         <v>0.9986720085144043</v>
       </c>
       <c r="AP12" t="n">
-        <v>0.9975685477256775</v>
+        <v>0.9975684285163879</v>
       </c>
       <c r="AQ12" t="n">
         <v>0.9960737824440002</v>

</xml_diff>